<commit_message>
working on the odd even predicates
</commit_message>
<xml_diff>
--- a/exp_results.xlsx
+++ b/exp_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahuis/Desktop/git/infer_TempDataLog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11AD67-D58C-3C4E-BE1F-22454F0C1877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FABA4A-6266-F94B-B16B-FFDB7CDA1D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="600" windowWidth="28960" windowHeight="17440" xr2:uid="{AB360DF6-4B39-8E4F-9F80-7BDD152B6CF2}"/>
   </bookViews>
@@ -222,17 +222,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,7 +551,7 @@
   <dimension ref="B3:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,32 +564,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
@@ -625,6 +625,9 @@
       <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="I5" s="1">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
@@ -765,32 +768,32 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="3" t="s">
         <v>24</v>
       </c>
@@ -828,7 +831,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="1">
@@ -851,7 +854,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="2">
@@ -874,7 +877,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="1">
@@ -943,7 +946,7 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="1">

</xml_diff>